<commit_message>
updates to supp files
</commit_message>
<xml_diff>
--- a/Supplementary Table 4.xlsx
+++ b/Supplementary Table 4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aldoa\OneDrive\Desktop\Prack ISME docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aldoa\OneDrive\Documents\GitHub\wyeomyia-niche-construction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2476CC0A-CB55-4C6D-BA7E-D7C9FE8B5DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4B5270-441E-42E3-85C8-8B08E8B397FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1170" windowWidth="29040" windowHeight="17520" xr2:uid="{493526D5-10F6-49C4-9B15-38A9903102B6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{493526D5-10F6-49C4-9B15-38A9903102B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="36">
   <si>
     <t>Comparison</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Model coefficient</t>
   </si>
   <si>
-    <t>&lt; 0.001</t>
-  </si>
-  <si>
     <t>Reference Level</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>&gt; 0.05</t>
-  </si>
-  <si>
     <t>Larvae vs start water (pooled)</t>
   </si>
   <si>
@@ -107,9 +101,6 @@
     <t>&lt;0.001***</t>
   </si>
   <si>
-    <t>0.001**</t>
-  </si>
-  <si>
     <t>Uncolonized</t>
   </si>
   <si>
@@ -147,6 +138,12 @@
   </si>
   <si>
     <t>Larvae-associated vs rearing water (High)</t>
+  </si>
+  <si>
+    <t>* p &lt; 0.05, ** p &lt; 0.01, *** p &lt; 0.001</t>
+  </si>
+  <si>
+    <t>&lt; 0.001 ***</t>
   </si>
 </sst>
 </file>
@@ -156,7 +153,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,16 +169,325 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -189,11 +495,159 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -211,9 +665,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -545,10 +1048,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3F61383-7624-434D-AD95-708238E2930A}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,19 +1069,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="6"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -594,7 +1097,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3"/>
@@ -605,62 +1108,62 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="E5" s="4">
         <v>-0.2</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="E6" s="4">
         <v>-0.25</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -671,7 +1174,7 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="3"/>
@@ -682,62 +1185,62 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1">
         <v>-4.4260000000000002</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" s="4">
         <v>-0.27700000000000002</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1">
         <v>-8.827</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E10" s="4">
         <v>-0.16200000000000001</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C11" s="4">
         <v>-4.4000000000000004</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E11" s="4">
         <v>0.1148</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -748,83 +1251,83 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>11</v>
+      <c r="A13" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="4">
         <v>-33.985999999999997</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E13" s="4">
         <v>-0.79600000000000004</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="4">
         <v>-37.858449999999998</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E14" s="4">
         <v>-0.90472759999999997</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="4">
         <v>-34.334969999999998</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E15" s="4">
         <v>-0.57770580000000005</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="1">
         <v>-29.3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E16" s="4">
         <v>-0.94281749999999998</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -835,7 +1338,7 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="3"/>
@@ -846,22 +1349,22 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -872,63 +1375,63 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="C21" s="4">
         <v>-10.407999999999999</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E21" s="4">
         <v>-0.247</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C22" s="4">
         <v>-10.624000000000001</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E22" s="4">
         <v>-0.13200000000000001</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C23" s="4">
         <v>-10.6</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E23" s="4">
         <v>-0.442</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -939,63 +1442,68 @@
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>15</v>
+      <c r="A25" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C25" s="4">
         <v>-23.55</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E25" s="4">
         <v>-0.54900000000000004</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C26" s="4">
         <v>-23.695509999999999</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E26" s="4">
         <v>-0.44543139999999998</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C27" s="4">
         <v>-18.74606</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E27" s="4">
         <v>-0.50063080000000004</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>